<commit_message>
Add course description and reqs on hover
</commit_message>
<xml_diff>
--- a/utils/data/audits-xlsx/cs-audit.xlsx
+++ b/utils/data/audits-xlsx/cs-audit.xlsx
@@ -2116,10 +2116,10 @@
     <t xml:space="preserve">ENGAGE in the Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">38-330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGAGE in Wellness: Looking Outward</t>
+    <t xml:space="preserve">38-230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGAGE in Wellness: Looking Inward</t>
   </si>
   <si>
     <t xml:space="preserve">38-430</t>
@@ -2612,7 +2612,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2641,12 +2641,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2698,7 +2692,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2708,10 +2702,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2907,10 +2897,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G507"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A308" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L340" activeCellId="0" sqref="L340"/>
+      <selection pane="topLeft" activeCell="A338" activeCellId="0" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9684,10 +9674,10 @@
       <c r="C337" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D337" s="3" t="s">
+      <c r="D337" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="G337" s="3" t="s">
+      <c r="G337" s="2" t="s">
         <v>678</v>
       </c>
     </row>
@@ -9701,10 +9691,10 @@
       <c r="C338" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="D338" s="3" t="s">
+      <c r="D338" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="G338" s="3" t="s">
+      <c r="G338" s="2" t="s">
         <v>678</v>
       </c>
     </row>
@@ -9718,10 +9708,10 @@
       <c r="C339" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="D339" s="3" t="s">
+      <c r="D339" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="G339" s="3" t="s">
+      <c r="G339" s="2" t="s">
         <v>678</v>
       </c>
     </row>
@@ -13091,6 +13081,7 @@
         <v>860</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>